<commit_message>
Completion of the file sending part via form
</commit_message>
<xml_diff>
--- a/storage/TCC.xlsx
+++ b/storage/TCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAE0215-ED5A-4D95-9C98-302759E91C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2AE0A1-C729-4DD5-9D8B-64E665CDE81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{522A90E7-3429-495C-95EA-772492626FA0}"/>
+    <workbookView xWindow="2415" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{522A90E7-3429-495C-95EA-772492626FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Coluna 1</t>
-  </si>
-  <si>
-    <t>Coluna 2</t>
-  </si>
-  <si>
-    <t>Coluna 3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>CET001</t>
   </si>
@@ -52,6 +43,27 @@
   </si>
   <si>
     <t>Transparencia</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>alo</t>
+  </si>
+  <si>
+    <t>figuras</t>
+  </si>
+  <si>
+    <t>Cod</t>
+  </si>
+  <si>
+    <t>Disciplina</t>
+  </si>
+  <si>
+    <t>Carga Horaria</t>
+  </si>
+  <si>
+    <t>Opcionais</t>
   </si>
 </sst>
 </file>
@@ -403,60 +415,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8EC18A-AD80-4927-B214-4C5473806A22}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>60</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>80</v>
       </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>